<commit_message>
Settings file added and read.
</commit_message>
<xml_diff>
--- a/FinansData.xlsx
+++ b/FinansData.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Aktier" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027" fullCalcOnLoad="1"/>
   <extLst>
@@ -25,27 +25,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Aktie beteckning</t>
   </si>
   <si>
-    <t>Slutkurs</t>
-  </si>
-  <si>
-    <t>Datumstämpel för inläsning</t>
+    <t xml:space="preserve">TradeDate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EarningsShare </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DaysLow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DaysHigh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastTradePriceOnly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open </t>
+  </si>
+  <si>
+    <t>DateStamp</t>
   </si>
   <si>
     <t>HM-B.ST</t>
   </si>
   <si>
-    <t>253.60</t>
+    <t>259.60</t>
+  </si>
+  <si>
+    <t>265.90</t>
+  </si>
+  <si>
+    <t>260.00</t>
   </si>
   <si>
     <t>VOLV-B.ST</t>
   </si>
   <si>
-    <t>97.05</t>
+    <t>7.17</t>
+  </si>
+  <si>
+    <t>95.55</t>
+  </si>
+  <si>
+    <t>97.25</t>
+  </si>
+  <si>
+    <t>96.10</t>
   </si>
   <si>
     <t>Namn</t>
@@ -57,7 +87,13 @@
     <t>Volvo B</t>
   </si>
   <si>
+    <t>Hämta förkortningen från https://finance.yahoo.com/</t>
+  </si>
+  <si>
     <t>HM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Där ser du också vilken data som kan hämtas. Endast den som har kolumner i Data arket sparas men modifikationer till programmet kan göras enkelt. </t>
   </si>
 </sst>
 </file>
@@ -67,8 +103,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,13 +136,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,12 +192,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabell2" displayName="Tabell2" ref="A1:C6" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabell2" displayName="Tabell2" ref="A1:H4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:H4"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Aktie beteckning"/>
-    <tableColumn id="2" name="Slutkurs"/>
-    <tableColumn id="3" name="Datumstämpel för inläsning" dataDxfId="0"/>
+    <tableColumn id="2" name="TradeDate "/>
+    <tableColumn id="3" name="EarningsShare "/>
+    <tableColumn id="4" name="DaysLow "/>
+    <tableColumn id="5" name="DaysHigh "/>
+    <tableColumn id="6" name="LastTradePriceOnly "/>
+    <tableColumn id="7" name="Open "/>
+    <tableColumn id="8" name="DateStamp" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -440,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -453,29 +518,56 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="F3:J5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <tableParts count="1">
@@ -486,50 +578,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.73046875" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="25.6640625" customWidth="1" style="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="14.86328125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="10.9296875" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="19.06640625" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="15" customWidth="1" style="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>42688.8317110417</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3">
+        <v>42691.6109973958</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>42688.8317085301</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3">
+        <v>42691.6109959722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>